<commit_message>
updated xls and doc
</commit_message>
<xml_diff>
--- a/goldberg_hornung_worszeck_sortout_timings.xlsx
+++ b/goldberg_hornung_worszeck_sortout_timings.xlsx
@@ -4,13 +4,16 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="20730" windowHeight="11760"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="19440" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_GoBack" localSheetId="0">Sheet1!$A$1</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
@@ -39,38 +42,63 @@
     <t>Release</t>
   </si>
   <si>
-    <t>v1</t>
-  </si>
-  <si>
-    <t>v2</t>
-  </si>
-  <si>
-    <t>total</t>
-  </si>
-  <si>
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>sortAll (fastest)</t>
-  </si>
-  <si>
-    <t>sortAll - 2 Threads</t>
-  </si>
-  <si>
-    <t>sortAll - 4 Threads</t>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>sortAll</t>
+  </si>
+  <si>
+    <t>MAPS Assignment 1: OpenMP Programming – Timings</t>
+  </si>
+  <si>
+    <t>v2 - SECTIONS</t>
+  </si>
+  <si>
+    <t>v1 - FOR</t>
+  </si>
+  <si>
+    <t>Goldberg, Peter | Hornung, Nico | Worszeck, Sascha | SHU 2012</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.00000000"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,11 +121,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -110,9 +146,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -150,7 +186,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -220,7 +256,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -394,109 +430,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:F38"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.85546875" customWidth="1"/>
+    <col min="5" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6">
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="B3" t="s">
+    <row r="1" spans="1:6" ht="20.25">
+      <c r="A1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="18">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E5" t="s">
         <v>5</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="10.5" customHeight="1"/>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="6" spans="1:6" ht="10.5" customHeight="1"/>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>11</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>3</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>4</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12">
-        <f>SUM(B5:B10)</f>
+        <v>4</v>
+      </c>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2">
+        <f>SUM(B7:B12)</f>
         <v>0</v>
       </c>
-      <c r="C12">
-        <f>SUM(C5:C10)</f>
+      <c r="C14" s="2">
+        <f>SUM(C7:C12)</f>
         <v>0</v>
       </c>
-      <c r="E12">
-        <f>SUM(E5:E10)</f>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2">
+        <f>SUM(E7:E12)</f>
         <v>0</v>
       </c>
-      <c r="F12">
-        <f>SUM(F5:F10)</f>
+      <c r="F14" s="2">
+        <f>SUM(F7:F12)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2">
-      <c r="B38" t="s">
-        <v>10</v>
+    <row r="37" spans="2:2">
+      <c r="B37" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -506,7 +583,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -518,7 +595,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added dual/quad-core timing sections
</commit_message>
<xml_diff>
--- a/goldberg_hornung_worszeck_sortout_timings.xlsx
+++ b/goldberg_hornung_worszeck_sortout_timings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>sortRows</t>
   </si>
@@ -61,6 +61,30 @@
   </si>
   <si>
     <t>Goldberg, Peter | Hornung, Nico | Worszeck, Sascha | SHU 2012</t>
+  </si>
+  <si>
+    <t>DualCore</t>
+  </si>
+  <si>
+    <t>QuadCore</t>
+  </si>
+  <si>
+    <t>Processor: Intel Core 2 Duo P7550 @ 2.26GHz</t>
+  </si>
+  <si>
+    <t>RAM: 4GB</t>
+  </si>
+  <si>
+    <t>OS: Windows 7 Professional (64-bit)</t>
+  </si>
+  <si>
+    <t>Processor: Intel Core i7-2600 @ 3.4GHz</t>
+  </si>
+  <si>
+    <t>RAM: 8GB</t>
+  </si>
+  <si>
+    <t>OS: Windows 7 Enterprise (64-bit)</t>
   </si>
 </sst>
 </file>
@@ -68,7 +92,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.00000000"/>
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -124,7 +148,7 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -430,144 +454,274 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2.85546875" customWidth="1"/>
     <col min="5" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" customWidth="1"/>
+    <col min="8" max="8" width="2.140625" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="11" max="12" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="2.85546875" customWidth="1"/>
+    <col min="14" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25">
+    <row r="1" spans="1:15" ht="20.25">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="18">
+    <row r="2" spans="1:15" ht="18">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="B4" s="1" t="s">
+    <row r="5" spans="1:15">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="B5" t="s">
+      <c r="K11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C12" t="s">
         <v>6</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E12" t="s">
         <v>5</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="10.5" customHeight="1"/>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
+      <c r="K12" t="s">
+        <v>5</v>
+      </c>
+      <c r="L12" t="s">
+        <v>6</v>
+      </c>
+      <c r="N12" t="s">
+        <v>5</v>
+      </c>
+      <c r="O12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="10.5" customHeight="1"/>
+    <row r="14" spans="1:15">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="J14" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="J15" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="J16" t="s">
+        <v>9</v>
+      </c>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="O16" s="2"/>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="J17" t="s">
+        <v>2</v>
+      </c>
+      <c r="K17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="O17" s="2"/>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="J18" t="s">
+        <v>3</v>
+      </c>
+      <c r="K18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="O18" s="2"/>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="J19" t="s">
+        <v>4</v>
+      </c>
+      <c r="K19" s="2"/>
+      <c r="L19" s="2"/>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+      <c r="O19" s="2"/>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="2">
-        <f>SUM(B7:B12)</f>
-        <v>0</v>
-      </c>
-      <c r="C14" s="2">
-        <f>SUM(C7:C12)</f>
-        <v>0</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2">
-        <f>SUM(E7:E12)</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="2">
-        <f>SUM(F7:F12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2">
-      <c r="B37" t="s">
+      <c r="B21" s="2">
+        <f>SUM(B14:B19)</f>
+        <v>0</v>
+      </c>
+      <c r="C21" s="2">
+        <f>SUM(C14:C19)</f>
+        <v>0</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2">
+        <f>SUM(E14:E19)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="2">
+        <f>SUM(F14:F19)</f>
+        <v>0</v>
+      </c>
+      <c r="J21" t="s">
+        <v>8</v>
+      </c>
+      <c r="K21" s="2">
+        <f>SUM(K14:K19)</f>
+        <v>0</v>
+      </c>
+      <c r="L21" s="2">
+        <f>SUM(L14:L19)</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2">
+        <f>SUM(N14:N19)</f>
+        <v>0</v>
+      </c>
+      <c r="O21" s="2">
+        <f>SUM(O14:O19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
+      <c r="B30" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Final Timings Nico is Gay
</commit_message>
<xml_diff>
--- a/goldberg_hornung_worszeck_sortout_timings.xlsx
+++ b/goldberg_hornung_worszeck_sortout_timings.xlsx
@@ -157,7 +157,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -170,9 +170,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -210,7 +210,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -280,7 +280,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -457,10 +457,10 @@
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
@@ -562,109 +562,205 @@
       <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
+      <c r="B14" s="2">
+        <v>0.35779300000000003</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.15864500000000001</v>
+      </c>
       <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="E14" s="2">
+        <v>0.47426600000000002</v>
+      </c>
+      <c r="F14" s="2">
+        <v>0.44431500000000002</v>
+      </c>
       <c r="J14" t="s">
         <v>0</v>
       </c>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
+      <c r="K14" s="2">
+        <v>9.5850699999999997E-2</v>
+      </c>
+      <c r="L14" s="2">
+        <v>4.7730300000000003E-2</v>
+      </c>
       <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
+      <c r="N14" s="2">
+        <v>0.17314599999999999</v>
+      </c>
+      <c r="O14" s="2">
+        <v>0.102475</v>
+      </c>
     </row>
     <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
+      <c r="B15" s="2">
+        <v>2.09293</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.26318999999999998</v>
+      </c>
       <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="E15" s="2">
+        <v>2.1465299999999998</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.31968600000000003</v>
+      </c>
       <c r="J15" t="s">
         <v>1</v>
       </c>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
+      <c r="K15" s="2">
+        <v>0.54662500000000003</v>
+      </c>
+      <c r="L15" s="2">
+        <v>9.8079600000000003E-2</v>
+      </c>
       <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
+      <c r="N15" s="2">
+        <v>1.47139</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0.16388900000000001</v>
+      </c>
     </row>
     <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>9</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="B16" s="2">
+        <v>0.247889</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.16555800000000001</v>
+      </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="E16" s="2">
+        <v>0.27794099999999999</v>
+      </c>
+      <c r="F16" s="2">
+        <v>0.17538999999999999</v>
+      </c>
       <c r="J16" t="s">
         <v>9</v>
       </c>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
+      <c r="K16" s="2">
+        <v>7.9160499999999995E-2</v>
+      </c>
+      <c r="L16" s="2">
+        <v>6.8063899999999997E-2</v>
+      </c>
       <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
+      <c r="N16" s="2">
+        <v>7.7828999999999995E-2</v>
+      </c>
+      <c r="O16" s="2">
+        <v>5.6844899999999997E-2</v>
+      </c>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="B17" s="2">
+        <v>1.74708</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.31976199999999999</v>
+      </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="E17" s="2">
+        <v>2.4739499999999999</v>
+      </c>
+      <c r="F17" s="2">
+        <v>0.31193399999999999</v>
+      </c>
       <c r="J17" t="s">
         <v>2</v>
       </c>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
+      <c r="K17" s="2">
+        <v>0.58961699999999995</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0.10283</v>
+      </c>
       <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
+      <c r="N17" s="2">
+        <v>1.28111</v>
+      </c>
+      <c r="O17" s="2">
+        <v>0.200625</v>
+      </c>
     </row>
     <row r="18" spans="1:15">
       <c r="A18" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
+      <c r="B18" s="2">
+        <v>0.42764400000000002</v>
+      </c>
+      <c r="C18" s="2">
+        <v>7.4173600000000006E-2</v>
+      </c>
       <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="E18" s="2">
+        <v>0.48702299999999998</v>
+      </c>
+      <c r="F18" s="2">
+        <v>9.77272E-2</v>
+      </c>
       <c r="J18" t="s">
         <v>3</v>
       </c>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
+      <c r="K18" s="2">
+        <v>0.112903</v>
+      </c>
+      <c r="L18" s="2">
+        <v>2.2629799999999999E-2</v>
+      </c>
       <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
+      <c r="N18" s="2">
+        <v>0.25892500000000002</v>
+      </c>
+      <c r="O18" s="2">
+        <v>4.34229E-2</v>
+      </c>
     </row>
     <row r="19" spans="1:15">
       <c r="A19" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="B19" s="2">
+        <v>1.9334</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.276758</v>
+      </c>
       <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="E19" s="2">
+        <v>2.1504099999999999</v>
+      </c>
+      <c r="F19" s="2">
+        <v>0.338003</v>
+      </c>
       <c r="J19" t="s">
         <v>4</v>
       </c>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
+      <c r="K19" s="2">
+        <v>0.62946500000000005</v>
+      </c>
+      <c r="L19" s="2">
+        <v>0.115315</v>
+      </c>
       <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
+      <c r="N19" s="2">
+        <v>1.2981199999999999</v>
+      </c>
+      <c r="O19" s="2">
+        <v>0.18610099999999999</v>
+      </c>
     </row>
     <row r="20" spans="1:15">
       <c r="B20" s="2"/>
@@ -684,40 +780,40 @@
       </c>
       <c r="B21" s="2">
         <f>SUM(B14:B19)</f>
-        <v>0</v>
+        <v>6.806735999999999</v>
       </c>
       <c r="C21" s="2">
         <f>SUM(C14:C19)</f>
-        <v>0</v>
+        <v>1.2580865999999999</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2">
         <f>SUM(E14:E19)</f>
-        <v>0</v>
+        <v>8.0101199999999988</v>
       </c>
       <c r="F21" s="2">
         <f>SUM(F14:F19)</f>
-        <v>0</v>
+        <v>1.6870552000000001</v>
       </c>
       <c r="J21" t="s">
         <v>8</v>
       </c>
       <c r="K21" s="2">
         <f>SUM(K14:K19)</f>
-        <v>0</v>
+        <v>2.0536211999999998</v>
       </c>
       <c r="L21" s="2">
         <f>SUM(L14:L19)</f>
-        <v>0</v>
+        <v>0.45464859999999996</v>
       </c>
       <c r="M21" s="2"/>
       <c r="N21" s="2">
         <f>SUM(N14:N19)</f>
-        <v>0</v>
+        <v>4.5605200000000004</v>
       </c>
       <c r="O21" s="2">
         <f>SUM(O14:O19)</f>
-        <v>0</v>
+        <v>0.75335779999999997</v>
       </c>
     </row>
     <row r="30" spans="1:15">
@@ -737,7 +833,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -749,7 +845,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>